<commit_message>
Se ajusta lógica de comprobantes contables y se ajustan parámetros de áreas a incluir
</commit_message>
<xml_diff>
--- a/static/TRN ÁGILES.xlsx
+++ b/static/TRN ÁGILES.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcastano\Documents\Rechazos\script\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorozco\Downloads\Aplicación rechazos depósitos\Aplicación rechazos depósitos\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB59F54-1858-4B4C-9EF3-85DBF81B8D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183656E0-74ED-42F1-AE08-CA70D199EB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4635" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{005EBF5A-5807-48EE-BA9B-69D36598620B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{005EBF5A-5807-48EE-BA9B-69D36598620B}"/>
   </bookViews>
   <sheets>
     <sheet name="Genérico" sheetId="1" r:id="rId1"/>
     <sheet name="BV" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BV!$A$2:$H$38</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="127">
   <si>
     <t>GENÉRICO</t>
   </si>
@@ -292,13 +295,139 @@
   </si>
   <si>
     <t>LECTURA BATCH</t>
+  </si>
+  <si>
+    <t>DT0023</t>
+  </si>
+  <si>
+    <t>DT0024</t>
+  </si>
+  <si>
+    <t>DT0025</t>
+  </si>
+  <si>
+    <t>DT0026</t>
+  </si>
+  <si>
+    <t>DT0027</t>
+  </si>
+  <si>
+    <t>DT0028</t>
+  </si>
+  <si>
+    <t>DT0029</t>
+  </si>
+  <si>
+    <t>DT0030</t>
+  </si>
+  <si>
+    <t>DT0031</t>
+  </si>
+  <si>
+    <t>DB  199095188  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  251005050  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  251005045  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  168795328  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  419595053  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  253095023  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  279505505  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  168795110  CR  210515020</t>
+  </si>
+  <si>
+    <t>DB  279505622  CR  210515020</t>
+  </si>
+  <si>
+    <t>OTRS.ACT.DIV.PROC.TARJ.OFICS.GCIAS.OP.ML</t>
+  </si>
+  <si>
+    <t>CXP.KTAL X PAGAR A REDEBAN CAJEROS RED</t>
+  </si>
+  <si>
+    <t>CXP KTAL X PAGAR A REDEBAN UTILIZ DATAFO</t>
+  </si>
+  <si>
+    <t>CXC DIVERSOS  PEAJE ELECTR CTA AHORROS Y CORRIENTE</t>
+  </si>
+  <si>
+    <t>OPERACIÓN INMOBILIARIA</t>
+  </si>
+  <si>
+    <t>COMERCIO INTERNACIONAL</t>
+  </si>
+  <si>
+    <t>SUFI</t>
+  </si>
+  <si>
+    <t>DIVERSOS OTROS LÍNEAS VIRTUALES CTA.CTE.IVA</t>
+  </si>
+  <si>
+    <t>GMF DESEMBOLSO CR A TERC GRAV</t>
+  </si>
+  <si>
+    <t>TEMP RECAUD CART HIPOT DESDE CTA AHORRO-CORRIENTE</t>
+  </si>
+  <si>
+    <t>CXC COMERCIO INTERNACIONAL COP</t>
+  </si>
+  <si>
+    <t>TEMP RECAUDOS OTRAS ENTIDADES SUFI-PAB</t>
+  </si>
+  <si>
+    <t>DT0034</t>
+  </si>
+  <si>
+    <t>CXC PARTIDAS DEBITO CB Y SUCURSALES</t>
+  </si>
+  <si>
+    <t>DB 168795024 CR 210515020</t>
+  </si>
+  <si>
+    <t>CAJEROS</t>
+  </si>
+  <si>
+    <t>SUCURSAL</t>
+  </si>
+  <si>
+    <t>CORRESPONSAL</t>
+  </si>
+  <si>
+    <t>CONTACT CENTER Y BPO</t>
+  </si>
+  <si>
+    <t>OPERACION DIGITAL</t>
+  </si>
+  <si>
+    <t>DT0010</t>
+  </si>
+  <si>
+    <t>DB  210515030  CR  210515020</t>
+  </si>
+  <si>
+    <t>EFECTIVO</t>
+  </si>
+  <si>
+    <t>AJUSTE DB CTA TEMPORAL DEPÓSITOS SUCURSALES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,12 +468,6 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -360,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -474,11 +597,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -564,20 +724,81 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -588,15 +809,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,6 +838,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{525AFDCA-1042-455F-80E7-DAA6F8A14F1D}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -938,13 +1177,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -1109,17 +1348,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BFB9646-70CE-401E-B052-09B612ADD72B}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.90625" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.36328125" bestFit="1" customWidth="1"/>
@@ -1127,16 +1366,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
     </row>
     <row r="2" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
@@ -1177,13 +1416,13 @@
       <c r="D3" s="14">
         <v>210515020</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="56">
         <v>145915122</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="58" t="s">
         <v>77</v>
       </c>
       <c r="H3" s="20"/>
@@ -1201,9 +1440,9 @@
       <c r="D4" s="18">
         <v>145915122</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="39"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="21">
         <v>10</v>
       </c>
@@ -1221,13 +1460,13 @@
       <c r="D5" s="25">
         <v>210515020</v>
       </c>
-      <c r="E5" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" s="35" t="s">
+      <c r="E5" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="58" t="s">
         <v>68</v>
       </c>
       <c r="H5" s="20"/>
@@ -1245,9 +1484,9 @@
       <c r="D6" s="26">
         <v>411525059</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="39"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1263,13 +1502,13 @@
       <c r="D7" s="14">
         <v>210515020</v>
       </c>
-      <c r="E7" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="35" t="s">
+      <c r="E7" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="64" t="s">
         <v>67</v>
       </c>
       <c r="H7" s="22"/>
@@ -1287,9 +1526,9 @@
       <c r="D8" s="17">
         <v>253500013</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="41"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="23">
         <v>994</v>
       </c>
@@ -1307,13 +1546,13 @@
       <c r="D9" s="25">
         <v>210515020</v>
       </c>
-      <c r="E9" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="35" t="s">
+      <c r="E9" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="64" t="s">
         <v>66</v>
       </c>
       <c r="H9" s="22"/>
@@ -1331,9 +1570,9 @@
       <c r="D10" s="26">
         <v>411525062</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="41"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="65"/>
       <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1349,13 +1588,13 @@
       <c r="D11" s="14">
         <v>210515020</v>
       </c>
-      <c r="E11" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="35" t="s">
+      <c r="E11" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="64" t="s">
         <v>65</v>
       </c>
       <c r="H11" s="22"/>
@@ -1373,9 +1612,9 @@
       <c r="D12" s="17">
         <v>253500012</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="41"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="65"/>
       <c r="H12" s="23">
         <v>994</v>
       </c>
@@ -1393,13 +1632,13 @@
       <c r="D13" s="25">
         <v>210515020</v>
       </c>
-      <c r="E13" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="35" t="s">
+      <c r="E13" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="40" t="s">
+      <c r="G13" s="64" t="s">
         <v>69</v>
       </c>
       <c r="H13" s="22"/>
@@ -1417,9 +1656,9 @@
       <c r="D14" s="26">
         <v>411525065</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="41"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="65"/>
       <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1435,13 +1674,13 @@
       <c r="D15" s="14">
         <v>210515020</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="35" t="s">
+      <c r="E15" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="58" t="s">
         <v>64</v>
       </c>
       <c r="H15" s="20"/>
@@ -1459,9 +1698,9 @@
       <c r="D16" s="18">
         <v>279505328</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="39"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="59"/>
       <c r="H16" s="21">
         <v>968</v>
       </c>
@@ -1476,16 +1715,16 @@
       <c r="C17" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="29">
         <v>210515020</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="56">
         <v>168795037</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="58" t="s">
         <v>77</v>
       </c>
       <c r="H17" s="20"/>
@@ -1500,12 +1739,12 @@
       <c r="C18" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="29">
         <v>168795037</v>
       </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="42"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="66"/>
       <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1518,14 +1757,14 @@
       <c r="C19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="29">
         <v>210515020</v>
       </c>
-      <c r="E19" s="37">
+      <c r="E19" s="60">
         <v>168795038</v>
       </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="42"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="66"/>
       <c r="H19" s="24"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1538,12 +1777,12 @@
       <c r="C20" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="29">
         <v>168795038</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="42"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="66"/>
       <c r="H20" s="24"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1556,14 +1795,14 @@
       <c r="C21" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="30">
+      <c r="D21" s="29">
         <v>210515020</v>
       </c>
-      <c r="E21" s="37">
+      <c r="E21" s="60">
         <v>168795036</v>
       </c>
-      <c r="F21" s="37"/>
-      <c r="G21" s="42"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="66"/>
       <c r="H21" s="24"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1576,33 +1815,35 @@
       <c r="C22" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="30">
+      <c r="D22" s="29">
         <v>168795036</v>
       </c>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="42"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="66"/>
       <c r="H22" s="24"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:8" s="50" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="29">
+      <c r="D23" s="48">
         <v>168795039</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="48">
         <v>168795039</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="23"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="49">
+        <v>968</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
@@ -1611,19 +1852,19 @@
       <c r="B24" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="30">
         <v>210515020</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="35" t="s">
+      <c r="E24" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="G24" s="38" t="s">
+      <c r="G24" s="58" t="s">
         <v>77</v>
       </c>
       <c r="H24" s="20"/>
@@ -1635,15 +1876,15 @@
       <c r="B25" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>210515050</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="39"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="59"/>
       <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1653,19 +1894,19 @@
       <c r="B26" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="31" t="s">
+      <c r="C26" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="30">
         <v>210515020</v>
       </c>
-      <c r="E26" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="35" t="s">
+      <c r="E26" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="56" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="38" t="s">
+      <c r="G26" s="58" t="s">
         <v>77</v>
       </c>
       <c r="H26" s="20"/>
@@ -1677,15 +1918,15 @@
       <c r="B27" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="32">
+      <c r="D27" s="31">
         <v>210515050</v>
       </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="39"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="59"/>
       <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1695,19 +1936,19 @@
       <c r="B28" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="31" t="s">
+      <c r="C28" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="30">
         <v>210515020</v>
       </c>
-      <c r="E28" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="F28" s="35" t="s">
+      <c r="E28" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="58" t="s">
         <v>77</v>
       </c>
       <c r="H28" s="20"/>
@@ -1719,22 +1960,389 @@
       <c r="B29" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="C29" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="32">
+      <c r="D29" s="31">
         <v>279505081</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="39"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="59"/>
       <c r="H29" s="21"/>
     </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="33">
+        <v>199095188</v>
+      </c>
+      <c r="E30" s="33">
+        <v>199095188</v>
+      </c>
+      <c r="F30" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="36">
+        <v>968</v>
+      </c>
+    </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="33"/>
+      <c r="A31" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="33">
+        <v>251005050</v>
+      </c>
+      <c r="E31" s="33">
+        <v>251005050</v>
+      </c>
+      <c r="F31" s="60"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="37">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="33">
+        <v>251005045</v>
+      </c>
+      <c r="E32" s="33">
+        <v>251005045</v>
+      </c>
+      <c r="F32" s="60"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="37">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="32">
+        <v>168795328</v>
+      </c>
+      <c r="E33" s="32">
+        <v>168795328</v>
+      </c>
+      <c r="F33" s="57"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="38">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D34" s="33">
+        <v>419595053</v>
+      </c>
+      <c r="E34" s="33">
+        <v>419595053</v>
+      </c>
+      <c r="F34" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="37"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="32">
+        <v>253095023</v>
+      </c>
+      <c r="E35" s="32">
+        <v>253095023</v>
+      </c>
+      <c r="F35" s="57"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="43">
+        <v>279505505</v>
+      </c>
+      <c r="E36" s="43">
+        <v>279505505</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="45">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="43">
+        <v>168795110</v>
+      </c>
+      <c r="E37" s="43">
+        <v>168795110</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G37" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H37" s="45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="52">
+        <v>279505622</v>
+      </c>
+      <c r="E38" s="52">
+        <v>279505622</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="H38" s="38">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D39" s="51">
+        <v>168795024</v>
+      </c>
+      <c r="E39" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="G39" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H39" s="23">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="51">
+        <v>168795024</v>
+      </c>
+      <c r="E40" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="G40" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H40" s="23">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="51">
+        <v>168795024</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="23">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="51">
+        <v>168795024</v>
+      </c>
+      <c r="E42" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="G42" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" s="51" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="51">
+        <v>168795024</v>
+      </c>
+      <c r="E43" s="51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G43" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="68" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="43">
+        <v>210515030</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="G44" s="69" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
+  <mergeCells count="40">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E6"/>
@@ -1756,17 +2364,21 @@
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="G17:G23"/>
+    <mergeCell ref="G30:G33"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E22"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="E13:E14"/>

</xml_diff>